<commit_message>
Added (MM/DD/YYYY) format to 'subscriber_list.xlsx' header
</commit_message>
<xml_diff>
--- a/subscriber_list.xlsx
+++ b/subscriber_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSR_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FB3461-D6FE-4CBE-ADE2-75157F2160FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76224238-636D-4324-997A-DEB0A6E4354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19710" yWindow="2610" windowWidth="28350" windowHeight="18225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,13 +30,13 @@
     <t>Subscriber ID</t>
   </si>
   <si>
-    <t>Subscriber Birth Date</t>
+    <t>Subscriber Birth Date (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Date of Issue</t>
+    <t>Date of Issue (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Date of Service</t>
+    <t>Date of Service (MM/DD/YYYY)</t>
   </si>
 </sst>
 </file>
@@ -387,15 +387,15 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>